<commit_message>
add name, manufacture number, part number, quantity, description, and id
</commit_message>
<xml_diff>
--- a/INVENTORY.xlsx
+++ b/INVENTORY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jub/work/KBL_INVENTORY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01397DDB-A995-964C-9202-EAC79EE25FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80B44D7-A0D8-A545-9CE8-68DF5C53EA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="840" windowWidth="28040" windowHeight="16440" xr2:uid="{37524684-4A0A-1D40-867A-AC342A308336}"/>
+    <workbookView xWindow="2140" yWindow="500" windowWidth="28040" windowHeight="16440" xr2:uid="{37524684-4A0A-1D40-867A-AC342A308336}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>quantity</t>
   </si>
@@ -50,12 +50,231 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>Green 573nm LED Indication - Discrete 1.95V 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>L171L-GC-TR</t>
+  </si>
+  <si>
+    <t>CKN10358-ND</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPST 25MA 24V</t>
+  </si>
+  <si>
+    <t>0805 GREEN SMD LED</t>
+  </si>
+  <si>
+    <t>manufacture_part_number</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>SDA01HSBD</t>
+  </si>
+  <si>
+    <t>Dip Switch SPST 1 Position Surface Mount Slide (Standard) Actuator 25mA 24VDC</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 2.54MM</t>
+  </si>
+  <si>
+    <t>PREC010SAAN-RC</t>
+  </si>
+  <si>
+    <t>S1012EC-10-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 10 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.02A 15V</t>
+  </si>
+  <si>
+    <t>EVQ-Q2YO3W</t>
+  </si>
+  <si>
+    <t>P12961SCT-ND</t>
+  </si>
+  <si>
+    <t>Tactile Switch SPST-NO Top Actuated Surface Mount</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD 20POS 2.54MM</t>
+  </si>
+  <si>
+    <t>3020-20-0300-00</t>
+  </si>
+  <si>
+    <t>1175-1623-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Surface Mount 20 position 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>CONN RCPT HSG 4POS 2.00MM</t>
+  </si>
+  <si>
+    <t>2CH-C-04</t>
+  </si>
+  <si>
+    <t>2057-2CH-C-04-ND</t>
+  </si>
+  <si>
+    <t>4 Rectangular Connectors - Housings Receptacle White 0.079" (2.00mm)</t>
+  </si>
+  <si>
+    <t>1528-1907-ND</t>
+  </si>
+  <si>
+    <t>MAGNETIC CONTACT SWITCH (DOOR SE)</t>
+  </si>
+  <si>
+    <t>Magnetic Reed Switch Magnet SPST-NO Wire Leads Rectangular, Wire Leads</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 30-26 AWG 2.00MM</t>
+  </si>
+  <si>
+    <t>2CTDC-R</t>
+  </si>
+  <si>
+    <t>2057-2CTDC-RCT-ND</t>
+  </si>
+  <si>
+    <t>Socket Contact Tin 22-28 AWG Crimp Stamped</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 100MA 6V</t>
+  </si>
+  <si>
+    <t>CJS-1200TA</t>
+  </si>
+  <si>
+    <t>563-1021-1-ND</t>
+  </si>
+  <si>
+    <t>Slide Switch SPDT Surface Mount</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 4POS 2MM</t>
+  </si>
+  <si>
+    <t>2SH-C-04-TR</t>
+  </si>
+  <si>
+    <t>2057-2SH-C-04-TR-ND</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole, Right Angle 4 position 0.079" (2.00mm)</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>GRM185R60J475ME15D</t>
+  </si>
+  <si>
+    <t>490-3892-1-ND</t>
+  </si>
+  <si>
+    <t>4.7 µF ±20% 6.3V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>10 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>CL10A225KQ8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1183-1-ND</t>
+  </si>
+  <si>
+    <t>2.2 µF ±10% 6.3V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>RES 82.5 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RMCF0805FT82R5</t>
+  </si>
+  <si>
+    <t>RMCF0805FT82R5CT-ND</t>
+  </si>
+  <si>
+    <t>82.5 Ohms ±1% 0.125W, 1/8W Chip Resistor 0805 (2012 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RES SMD 110 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RC080FR-07110RL</t>
+  </si>
+  <si>
+    <t>311-110CRCT-ND</t>
+  </si>
+  <si>
+    <t>110 Ohms ±1% 0.125W, 1/8W Chip Resistor 0805 (2012 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>LCD DISP TF 2.4' 240X320</t>
+  </si>
+  <si>
+    <t>NHD-2.4-240320CF-CTXI#-FT</t>
+  </si>
+  <si>
+    <t>NHD-2.4-240320CF-CTXI#-FT-ND</t>
+  </si>
+  <si>
+    <t>Resistive Graphic LCD Display Module Transmissive Red, Green, Blue (RGB) TFT - Color Parallel, 8-Bit/16-Bit (RGB) 2.4" (60.96mm) 240 x 320</t>
+  </si>
+  <si>
+    <t>DIODE GEN PURP 100V 300MA SOD123</t>
+  </si>
+  <si>
+    <t>IN4148W-7-F</t>
+  </si>
+  <si>
+    <t>1N4148W-FDICT-ND</t>
+  </si>
+  <si>
+    <t>Diode Standard 100 V 300mA (DC) Surface Mount SOD-123</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 8KB FLASH 20TSSOP</t>
+  </si>
+  <si>
+    <t>STM32L011F3P6</t>
+  </si>
+  <si>
+    <t>497-17476-ND</t>
+  </si>
+  <si>
+    <t>ARM® Cortex®-M0+ series Microcontroller IC 32-Bit 32MHz 8KB (8K x 8) FLASH 20-TSSOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -93,10 +312,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,32 +654,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E449FA4-42FC-444E-8B1F-FF9487B9E5F9}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="12.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>95</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2">
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="6">
+        <v>375</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="2">
+        <v>96</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2">
+        <v>79</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+    <sortCondition ref="B2:B20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>